<commit_message>
update to latest files
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rakes\eclipse-workspace\SeleniumDemo\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github-workspace\SeleniumDemo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4E582E-1847-4323-B529-EB879758DF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EA31CC-4105-4227-9099-2BD44A774AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A5C82274-9192-450A-A529-6BA59D7B56D7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Dha1357#</t>
+  </si>
+  <si>
+    <t>dhanya.com</t>
+  </si>
+  <si>
+    <t>Dhan</t>
   </si>
 </sst>
 </file>
@@ -410,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8833BF-20B6-4269-9CF6-6F16C9ACAA67}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,6 +443,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{2916F9E7-85F5-4D2C-B24E-246C8A734776}"/>

</xml_diff>